<commit_message>
Updated the Self Assessment
</commit_message>
<xml_diff>
--- a/PI-2023-24 Self-Assessment.xlsx
+++ b/PI-2023-24 Self-Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoãoTeixeira(1180590\Desktop\entrega\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Erasmus\PPROG\lei-24-s2-1de_e-g055\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAFBD6A-DA67-40F9-99B3-659D44C45A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE17880B-07C3-4388-ADC4-77CD33943F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="138">
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -66,12 +66,6 @@
   </si>
   <si>
     <t>List A</t>
-  </si>
-  <si>
-    <t>Student 5</t>
-  </si>
-  <si>
-    <t>Student 6</t>
   </si>
   <si>
     <t>Student 7</t>
@@ -1213,6 +1207,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1243,11 +1238,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Százalék" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -1779,76 +1773,76 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:T36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.59765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.875" customWidth="1"/>
+    <col min="4" max="19" width="7.8984375" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:20" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:20" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="67"/>
-    </row>
-    <row r="9" spans="1:20" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+      <c r="I8" s="67"/>
+      <c r="J8" s="67"/>
+      <c r="K8" s="67"/>
+      <c r="L8" s="67"/>
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="67"/>
+      <c r="P8" s="67"/>
+      <c r="Q8" s="67"/>
+      <c r="R8" s="67"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="68"/>
+    </row>
+    <row r="9" spans="1:20" ht="105.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="42">
@@ -1867,13 +1861,13 @@
         <f>C13</f>
         <v>1232225</v>
       </c>
-      <c r="H9" s="43" t="str">
+      <c r="H9" s="43">
         <f>C14</f>
-        <v>Student 5</v>
-      </c>
-      <c r="I9" s="43" t="str">
+        <v>1232250</v>
+      </c>
+      <c r="I9" s="43">
         <f>C15</f>
-        <v>Student 6</v>
+        <v>1232233</v>
       </c>
       <c r="J9" s="43" t="str">
         <f>C16</f>
@@ -1915,8 +1909,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="62" t="s">
+    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="63" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="37">
@@ -1948,8 +1942,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="63"/>
+    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="64"/>
       <c r="C11" s="8">
         <v>1232296</v>
       </c>
@@ -1979,8 +1973,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="63"/>
+    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="64"/>
       <c r="C12" s="8">
         <v>1232216</v>
       </c>
@@ -2010,17 +2004,29 @@
         <v>4.333333333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="63"/>
+    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="64"/>
       <c r="C13" s="8">
         <v>1232225</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="8"/>
+      <c r="D13" s="8">
+        <v>5</v>
+      </c>
+      <c r="E13" s="8">
+        <v>5</v>
+      </c>
+      <c r="F13" s="9">
+        <v>5</v>
+      </c>
+      <c r="G13" s="36">
+        <v>5</v>
+      </c>
+      <c r="H13" s="35">
+        <v>5</v>
+      </c>
+      <c r="I13" s="8">
+        <v>5</v>
+      </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8"/>
@@ -2030,15 +2036,15 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="10"/>
-      <c r="S13" s="51" t="e">
+      <c r="S13" s="51">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="63"/>
-      <c r="C14" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="64"/>
+      <c r="C14" s="8">
+        <v>1232250</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -2060,10 +2066,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="63"/>
-      <c r="C15" s="8" t="s">
-        <v>8</v>
+    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="64"/>
+      <c r="C15" s="8">
+        <v>1232233</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -2085,10 +2091,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="63"/>
+    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="64"/>
       <c r="C16" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -2110,10 +2116,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="63"/>
+    <row r="17" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="64"/>
       <c r="C17" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -2135,10 +2141,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="63"/>
+    <row r="18" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="64"/>
       <c r="C18" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
@@ -2160,10 +2166,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="63"/>
+    <row r="19" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="64"/>
       <c r="C19" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2185,10 +2191,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="63"/>
+    <row r="20" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="64"/>
       <c r="C20" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
@@ -2210,10 +2216,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="63"/>
+    <row r="21" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="64"/>
       <c r="C21" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -2235,10 +2241,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="63"/>
+    <row r="22" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="64"/>
       <c r="C22" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -2260,10 +2266,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="63"/>
+    <row r="23" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="64"/>
       <c r="C23" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -2285,10 +2291,10 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="64"/>
+    <row r="24" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="65"/>
       <c r="C24" s="40" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D24" s="40"/>
       <c r="E24" s="40"/>
@@ -2310,7 +2316,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="45" t="s">
         <v>5</v>
@@ -2325,19 +2331,19 @@
       </c>
       <c r="F25" s="46">
         <f t="shared" si="1"/>
-        <v>4.333333333333333</v>
-      </c>
-      <c r="G25" s="46" t="e">
+        <v>4.5</v>
+      </c>
+      <c r="G25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H25" s="46" t="e">
+        <v>5</v>
+      </c>
+      <c r="H25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I25" s="46" t="e">
+        <v>5</v>
+      </c>
+      <c r="I25" s="46">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>5</v>
       </c>
       <c r="J25" s="46" t="e">
         <f t="shared" si="1"/>
@@ -2377,74 +2383,74 @@
       </c>
       <c r="S25" s="53"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>0</v>
-      </c>
-      <c r="B31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
-      </c>
-      <c r="E36" s="72"/>
+        <v>25</v>
+      </c>
+      <c r="E36" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2466,36 +2472,36 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
     <col min="5" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="71" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="C3" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="D3" s="69" t="s">
         <v>30</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="68" t="s">
-        <v>32</v>
       </c>
       <c r="E3" s="11">
         <v>0</v>
@@ -2516,55 +2522,55 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="69"/>
+    <row r="4" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="64"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="70"/>
       <c r="E4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="H4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="I4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="J4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="7" t="s">
+    </row>
+    <row r="5" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="64"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="F5" s="23" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="22" t="s">
+      <c r="G5" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="H5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="I5" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="J5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>1</v>
       </c>
@@ -2576,25 +2582,25 @@
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="32" t="s">
+      <c r="H6" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="I6" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="32" t="s">
+      <c r="J6" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>2</v>
       </c>
@@ -2606,25 +2612,25 @@
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="7" t="s">
+      <c r="J7" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>3</v>
       </c>
@@ -2636,25 +2642,25 @@
       </c>
       <c r="D8" s="60"/>
       <c r="E8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="H8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J8" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>4</v>
       </c>
@@ -2666,25 +2672,25 @@
       </c>
       <c r="D9" s="60"/>
       <c r="E9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="H9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="I9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
         <v>5</v>
       </c>
@@ -2696,382 +2702,382 @@
       </c>
       <c r="D10" s="60"/>
       <c r="E10" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="J10" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J10" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="60"/>
       <c r="E11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="I11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="7" t="s">
+      <c r="J11" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="60"/>
       <c r="E12" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="H12" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="I12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="7" t="s">
+      <c r="J12" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="60"/>
       <c r="E13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="I13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="7" t="s">
+      <c r="J13" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J13" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="60"/>
       <c r="E14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="H14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="I14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="7" t="s">
+      <c r="J14" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J14" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="60"/>
       <c r="E15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="I15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" s="7" t="s">
+      <c r="J15" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
       <c r="D16" s="60"/>
       <c r="E16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="H16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="7" t="s">
+      <c r="J16" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J16" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="60"/>
       <c r="E17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="H17" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="I17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" s="7" t="s">
+      <c r="J17" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J17" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="60"/>
       <c r="E18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="H18" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="I18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="7" t="s">
+      <c r="J18" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="60"/>
       <c r="E19" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="H19" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I19" s="7" t="s">
+      <c r="J19" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="60"/>
       <c r="E20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="H20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="I20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I20" s="7" t="s">
+      <c r="J20" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="60"/>
       <c r="E21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="I21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I21" s="7" t="s">
+      <c r="J21" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="60"/>
       <c r="E22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="H22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="I22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="J22" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J22" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="60"/>
       <c r="E23" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="I23" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H23" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="7" t="s">
+      <c r="J23" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J23" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="60"/>
       <c r="E24" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="I24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H24" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="I24" s="7" t="s">
+      <c r="J24" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="J24" s="33" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:10" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="22"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54"/>
       <c r="D25" s="61"/>
       <c r="E25" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="23" t="s">
+      <c r="H25" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G25" s="23" t="s">
+      <c r="I25" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="I25" s="23" t="s">
+      <c r="J25" s="33" t="s">
         <v>43</v>
-      </c>
-      <c r="J25" s="33" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3119,26 +3125,26 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -3155,13 +3161,13 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="2" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
@@ -3179,13 +3185,13 @@
         <f>'Group and Self Assessment'!C13</f>
         <v>1232225</v>
       </c>
-      <c r="G3" s="20" t="str">
+      <c r="G3" s="20">
         <f>'Group and Self Assessment'!C14</f>
-        <v>Student 5</v>
-      </c>
-      <c r="H3" s="20" t="str">
+        <v>1232250</v>
+      </c>
+      <c r="H3" s="20">
         <f>'Group and Self Assessment'!C15</f>
-        <v>Student 6</v>
+        <v>1232233</v>
       </c>
       <c r="I3" s="20" t="str">
         <f>'Group and Self Assessment'!C16</f>
@@ -3251,15 +3257,15 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
@@ -3290,29 +3296,29 @@
         <v>5</v>
       </c>
       <c r="S4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="T4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="V4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="U4" s="7" t="s">
+      <c r="W4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="V4" s="7" t="s">
+      <c r="X4" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="Y4" s="7"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="17">
         <v>0.2</v>
@@ -3343,29 +3349,29 @@
         <v>4</v>
       </c>
       <c r="S5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="V5" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="W5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="X5" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="W5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="X5" s="7" t="s">
-        <v>64</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="78" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="17">
         <v>0.5</v>
@@ -3396,29 +3402,29 @@
         <v>4</v>
       </c>
       <c r="S6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="V6" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="W6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="V6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="W6" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="X6" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Y6" s="7"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="17">
         <v>0.2</v>
@@ -3443,29 +3449,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="U7" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="T7" s="7" t="s">
+      <c r="V7" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="U7" s="7" t="s">
+      <c r="W7" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="V7" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="W7" s="7" t="s">
-        <v>76</v>
-      </c>
       <c r="X7" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Y7" s="7"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
@@ -3541,9 +3547,9 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23">
@@ -3616,7 +3622,7 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="16"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
   </sheetData>
@@ -3639,24 +3645,24 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="17" width="5.625" style="1" customWidth="1"/>
-    <col min="18" max="18" width="12.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="5.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="20.625" style="1" customWidth="1"/>
+    <col min="22" max="24" width="20.59765625" style="1" customWidth="1"/>
     <col min="25" max="25" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.875" style="1"/>
+    <col min="26" max="26" width="8.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="7.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="13"/>
@@ -3673,12 +3679,12 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
     </row>
-    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="57" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="20">
         <f>'Group and Self Assessment'!C10</f>
@@ -3696,13 +3702,13 @@
         <f>'Group and Self Assessment'!C13</f>
         <v>1232225</v>
       </c>
-      <c r="G3" s="20" t="str">
+      <c r="G3" s="20">
         <f>'Group and Self Assessment'!C14</f>
-        <v>Student 5</v>
-      </c>
-      <c r="H3" s="20" t="str">
+        <v>1232250</v>
+      </c>
+      <c r="H3" s="20">
         <f>'Group and Self Assessment'!C15</f>
-        <v>Student 6</v>
+        <v>1232233</v>
       </c>
       <c r="I3" s="20" t="str">
         <f>'Group and Self Assessment'!C16</f>
@@ -3768,15 +3774,15 @@
         <v>5</v>
       </c>
       <c r="Y3" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="144.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="17">
         <v>0.1</v>
@@ -3801,29 +3807,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S4" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="U4" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="T4" s="59" t="s">
+      <c r="V4" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="U4" s="59" t="s">
+      <c r="W4" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="V4" s="59" t="s">
+      <c r="X4" s="59" t="s">
         <v>83</v>
-      </c>
-      <c r="W4" s="59" t="s">
-        <v>84</v>
-      </c>
-      <c r="X4" s="59" t="s">
-        <v>85</v>
       </c>
       <c r="Y4" s="56"/>
       <c r="Z4" s="15"/>
     </row>
-    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="101.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B5" s="17">
         <v>0.1</v>
@@ -3848,29 +3854,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S5" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="T5" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="U5" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="T5" s="59" t="s">
+      <c r="V5" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="U5" s="59" t="s">
+      <c r="W5" s="59" t="s">
         <v>89</v>
       </c>
-      <c r="V5" s="59" t="s">
+      <c r="X5" s="59" t="s">
         <v>90</v>
-      </c>
-      <c r="W5" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="X5" s="59" t="s">
-        <v>92</v>
       </c>
       <c r="Y5" s="56"/>
       <c r="Z5" s="15"/>
     </row>
-    <row r="6" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B6" s="17">
         <v>0.05</v>
@@ -3895,29 +3901,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S6" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="T6" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="U6" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="T6" s="59" t="s">
+      <c r="V6" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="U6" s="59" t="s">
+      <c r="W6" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="V6" s="59" t="s">
+      <c r="X6" s="59" t="s">
         <v>97</v>
-      </c>
-      <c r="W6" s="59" t="s">
-        <v>98</v>
-      </c>
-      <c r="X6" s="59" t="s">
-        <v>99</v>
       </c>
       <c r="Y6" s="56"/>
       <c r="Z6" s="15"/>
     </row>
-    <row r="7" spans="1:26" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B7" s="17">
         <v>0.05</v>
@@ -3942,29 +3948,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S7" s="59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T7" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="U7" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="V7" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="U7" s="59" t="s">
+      <c r="W7" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="V7" s="59" t="s">
+      <c r="X7" s="59" t="s">
         <v>103</v>
-      </c>
-      <c r="W7" s="59" t="s">
-        <v>104</v>
-      </c>
-      <c r="X7" s="59" t="s">
-        <v>105</v>
       </c>
       <c r="Y7" s="56"/>
       <c r="Z7" s="15"/>
     </row>
-    <row r="8" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B8" s="17">
         <v>0.1</v>
@@ -3989,29 +3995,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S8" s="59" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T8" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="U8" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="V8" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="U8" s="59" t="s">
+      <c r="W8" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="V8" s="59" t="s">
+      <c r="X8" s="59" t="s">
         <v>109</v>
-      </c>
-      <c r="W8" s="59" t="s">
-        <v>110</v>
-      </c>
-      <c r="X8" s="59" t="s">
-        <v>111</v>
       </c>
       <c r="Y8" s="56"/>
       <c r="Z8" s="15"/>
     </row>
-    <row r="9" spans="1:26" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9" s="17">
         <v>0.05</v>
@@ -4036,25 +4042,25 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S9" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T9" s="59" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="U9" s="59"/>
       <c r="V9" s="59" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="W9" s="59"/>
       <c r="X9" s="59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Y9" s="56"/>
       <c r="Z9" s="15"/>
     </row>
-    <row r="10" spans="1:26" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="17">
         <v>0.1</v>
@@ -4079,29 +4085,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S10" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T10" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="U10" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="V10" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="U10" s="59" t="s">
+      <c r="W10" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="V10" s="59" t="s">
+      <c r="X10" s="59" t="s">
         <v>120</v>
-      </c>
-      <c r="W10" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="X10" s="59" t="s">
-        <v>122</v>
       </c>
       <c r="Y10" s="56"/>
       <c r="Z10" s="15"/>
     </row>
-    <row r="11" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B11" s="17">
         <v>0.1</v>
@@ -4126,29 +4132,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S11" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T11" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="U11" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="V11" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U11" s="59" t="s">
+      <c r="W11" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="V11" s="59" t="s">
+      <c r="X11" s="59" t="s">
         <v>126</v>
-      </c>
-      <c r="W11" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="X11" s="59" t="s">
-        <v>128</v>
       </c>
       <c r="Y11" s="56"/>
       <c r="Z11" s="15"/>
     </row>
-    <row r="12" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B12" s="17">
         <v>0.1</v>
@@ -4173,29 +4179,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S12" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T12" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="U12" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="V12" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U12" s="59" t="s">
+      <c r="W12" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="V12" s="59" t="s">
+      <c r="X12" s="59" t="s">
         <v>126</v>
-      </c>
-      <c r="W12" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="X12" s="59" t="s">
-        <v>128</v>
       </c>
       <c r="Y12" s="56"/>
       <c r="Z12" s="15"/>
     </row>
-    <row r="13" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B13" s="17">
         <v>0.1</v>
@@ -4220,29 +4226,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S13" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="T13" s="59" t="s">
+        <v>130</v>
+      </c>
+      <c r="U13" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="T13" s="59" t="s">
+      <c r="V13" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="U13" s="59" t="s">
+      <c r="W13" s="59" t="s">
         <v>133</v>
       </c>
-      <c r="V13" s="59" t="s">
+      <c r="X13" s="59" t="s">
         <v>134</v>
-      </c>
-      <c r="W13" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="X13" s="59" t="s">
-        <v>136</v>
       </c>
       <c r="Y13" s="56"/>
       <c r="Z13" s="15"/>
     </row>
-    <row r="14" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B14" s="17">
         <v>0.15</v>
@@ -4267,29 +4273,29 @@
         <v>#DIV/0!</v>
       </c>
       <c r="S14" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="T14" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="U14" s="59" t="s">
+        <v>123</v>
+      </c>
+      <c r="V14" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="U14" s="59" t="s">
+      <c r="W14" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="V14" s="59" t="s">
+      <c r="X14" s="59" t="s">
         <v>126</v>
-      </c>
-      <c r="W14" s="59" t="s">
-        <v>127</v>
-      </c>
-      <c r="X14" s="59" t="s">
-        <v>128</v>
       </c>
       <c r="Y14" s="56"/>
       <c r="Z14" s="15"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B15" s="18">
         <f>SUM(B4:B14)</f>
@@ -4365,9 +4371,9 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="15"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23">
@@ -4440,7 +4446,7 @@
       <c r="Y16" s="23"/>
       <c r="Z16" s="16"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
@@ -4455,6 +4461,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9d21ddf3f0b128e39c9d770c8c903166">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0326308c339679ad994635f2c691325" ns2:_="">
     <xsd:import namespace="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
@@ -4638,22 +4659,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B77F7C-EE47-4FBD-B078-6536C1487A1E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4669,28 +4699,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F61419B8-A98A-41CD-95EE-48A4F975B8D1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D8D82CB-2E6F-4A14-B6B4-DFDD1BBD70FC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>